<commit_message>
save rpg and sql and clone
</commit_message>
<xml_diff>
--- a/rpg_lib.xlsx
+++ b/rpg_lib.xlsx
@@ -13,14 +13,14 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$52</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
   <si>
     <t>Language</t>
   </si>
@@ -223,9 +223,6 @@
 C     VAR_B         DSPLY                                  
 C                   ENDSR                                  
 ****************** End of data ****************************</t>
-  </si>
-  <si>
-    <t>Sub Routine</t>
   </si>
   <si>
     <t xml:space="preserve"> * Define the target file                                                 
@@ -717,9 +714,6 @@
     </r>
   </si>
   <si>
-    <t>chain</t>
-  </si>
-  <si>
     <t xml:space="preserve">0002.00 FLNSTPARM  IF   E           K DISK                                 
 0003.00 DKEY              S              3P 0                              
 0004.00 DCHK              S              1P 0                              
@@ -732,15 +726,6 @@
 0011.00 C     CHK           DSPLY                                          
 0012.00 C                   SETON                                        LR
 0013.00 C                   RETURN                                         </t>
-  </si>
-  <si>
-    <t>loop file in sr/ setll</t>
-  </si>
-  <si>
-    <t>chain 連鎖</t>
-  </si>
-  <si>
-    <t>chain keylist</t>
   </si>
   <si>
     <t xml:space="preserve">0081.00 C     KCUP009LT     CHAIN     CUP009LT                           88 
@@ -776,9 +761,6 @@
     <t>EDITC</t>
   </si>
   <si>
-    <t>Procedure</t>
-  </si>
-  <si>
     <t>Short-cut</t>
   </si>
   <si>
@@ -815,9 +797,6 @@
 0603.00 C/COPY CFSORC,SRP012  
 0604.00 C/COPY CFSORC,SRP019  
 0605.00 C/COPY CFSORC,SRP005  </t>
-  </si>
-  <si>
-    <t>copy official source (I700BS/CFSORC)</t>
   </si>
   <si>
     <t>* All the 101 records in ORDFIL are to be printed. The value 101
@@ -863,6 +842,39 @@
   </si>
   <si>
     <t>像莎翁的十四行詩一樣華麗的RPG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     C                   Z-ADD     1             BANK              3 0
+     C                   MOVE      '1'           RECTYP            1
+     C                   Z-ADD     20            APLNO             2 0
+      *CUP009 key.
+     C     KEY009        KLIST
+     C                   KFLD                    BANK
+     C                   KFLD                    RECTYP
+     C                   KFLD                    PCIF</t>
+  </si>
+  <si>
+    <t>KLIST</t>
+  </si>
+  <si>
+    <t>CHAIN</t>
+  </si>
+  <si>
+    <t>PLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     C     *ENTRY        PLIST
+     C                   PARM                    PCIF             10
+     C                   PARM                    PIS_EMP           1</t>
+  </si>
+  <si>
+    <t>COPY (I700BS/CFSORC)</t>
+  </si>
+  <si>
+    <t>SETLL, *START</t>
+  </si>
+  <si>
+    <t>EXSR</t>
   </si>
 </sst>
 </file>
@@ -1248,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1"/>
@@ -1278,7 +1290,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -1289,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
@@ -1399,7 +1411,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>23</v>
@@ -1410,10 +1422,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="26.25" customHeight="1">
@@ -1421,10 +1433,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="26.25" customHeight="1">
@@ -1432,10 +1444,10 @@
         <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.25" customHeight="1">
@@ -1443,10 +1455,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.25" customHeight="1">
@@ -1454,43 +1466,43 @@
         <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.25" customHeight="1">
       <c r="A19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.25" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.25" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.25" customHeight="1">
@@ -1498,10 +1510,10 @@
         <v>3</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.25" customHeight="1">
@@ -1509,38 +1521,38 @@
         <v>3</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.25" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.25" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.25" customHeight="1">
@@ -1548,52 +1560,52 @@
         <v>3</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.25" customHeight="1">
       <c r="A27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.25" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.25" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.25" customHeight="1">
@@ -1601,10 +1613,10 @@
         <v>3</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.25" customHeight="1">
@@ -1612,10 +1624,10 @@
         <v>3</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.25" customHeight="1">
@@ -1623,10 +1635,10 @@
         <v>3</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="26.25" customHeight="1">
@@ -1634,10 +1646,10 @@
         <v>3</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="26.25" customHeight="1">
@@ -1645,10 +1657,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="26.25" customHeight="1">
@@ -1656,10 +1668,10 @@
         <v>3</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="26.25" customHeight="1">
@@ -1667,10 +1679,10 @@
         <v>3</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="26.25" customHeight="1">
@@ -1678,10 +1690,10 @@
         <v>3</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="26.25" customHeight="1">
@@ -1689,10 +1701,10 @@
         <v>3</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="26.25" customHeight="1">
@@ -1700,19 +1712,21 @@
         <v>3</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="40" spans="1:3" ht="26.25" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="26.25" customHeight="1">
@@ -1720,30 +1734,41 @@
         <v>3</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="11.25">
+      <c r="A42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="26.25" customHeight="1">
+      <c r="A43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="26.25" customHeight="1">
-      <c r="A42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="26.25" customHeight="1">
+      <c r="A44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="26.25" customHeight="1">
-      <c r="C43" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="26.25" customHeight="1">
-      <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" ht="26.25" customHeight="1">
       <c r="C45" s="4"/>
@@ -1757,17 +1782,14 @@
     <row r="48" spans="1:3" ht="26.25" customHeight="1">
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="3:3" ht="26.25" customHeight="1">
-      <c r="C49" s="4"/>
+    <row r="50" spans="3:3" ht="26.25" customHeight="1">
+      <c r="C50" s="4"/>
     </row>
     <row r="51" spans="3:3" ht="26.25" customHeight="1">
       <c r="C51" s="4"/>
     </row>
     <row r="52" spans="3:3" ht="26.25" customHeight="1">
       <c r="C52" s="4"/>
-    </row>
-    <row r="53" spans="3:3" ht="26.25" customHeight="1">
-      <c r="C53" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add rpglib about PF and LF of a pf in 1 program.
</commit_message>
<xml_diff>
--- a/rpg_lib.xlsx
+++ b/rpg_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="105">
   <si>
     <t>Language</t>
   </si>
@@ -963,6 +963,17 @@
     <t xml:space="preserve">C     *DTAARA       DEFINE                  EXDCAPPRM        32     
 C                   IN        *DTAARA                               
 C     EXDCAPPRM     DSPLY                                           </t>
+  </si>
+  <si>
+    <t>PF and LF in same program</t>
+  </si>
+  <si>
+    <t>FACADBFSS  IF   E           K DISK                              
+FFSSDBWRK  UF A E           K DISK                                    
+FFSSDBWRKLFUF A E           K DISK    PREFIX('X')                     
+F                                     RENAME(RFSSDBWRK:RLF)           
+...
+Please reference  ZAUTOPAY/QFSSSRC (FSSGDBPTY )</t>
   </si>
 </sst>
 </file>
@@ -1350,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1"/>
@@ -1914,7 +1925,15 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="26.25" customHeight="1">
-      <c r="C50" s="4"/>
+      <c r="A50" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="51" spans="1:3" ht="26.25" customHeight="1">
       <c r="C51" s="4"/>

</xml_diff>

<commit_message>
Add rpg entries about array define, %lookup and how to fold/unfold subfile
</commit_message>
<xml_diff>
--- a/rpg_lib.xlsx
+++ b/rpg_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="111">
   <si>
     <t>Language</t>
   </si>
@@ -974,6 +974,118 @@
 F                                     RENAME(RFSSDBWRK:RLF)           
 ...
 Please reference  ZAUTOPAY/QFSSSRC (FSSGDBPTY )</t>
+  </si>
+  <si>
+    <t>Array define in old format</t>
+  </si>
+  <si>
+    <t>Look up array built-in function</t>
+  </si>
+  <si>
+    <t>Fold/Unfold</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Define the dds like this (multiple line is allowed)
+A            DCCY           3   O </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">61                   
+A            DAMT          13  2O  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 65EDTCDE(P)                    
+A            DDTE           6  0O </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 19EDTWRD('  /  /  ') 
+A            DTIM           6  0O </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 9 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>28EDTWRD('  :  :  ') 
+2. Add keyword to subfile control record
+SFLPAG(0006)    //size when unfold
+...
+SFLDROP(CF20)   //assign f20 to the control framework</t>
+    </r>
+  </si>
+  <si>
+    <t>mylesDVSOWNREL         S              3    DIM(10) CTDATA
+…
+mylesC**             //program end
+SOW
+OWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%LOOKUP(CUXREL:VSOWNREL) &lt;&gt; 0  </t>
   </si>
 </sst>
 </file>
@@ -1359,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1"/>
@@ -1936,10 +2048,37 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="26.25" customHeight="1">
-      <c r="C51" s="4"/>
+      <c r="A51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="52" spans="1:3" ht="26.25" customHeight="1">
-      <c r="C52" s="4"/>
+      <c r="A52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="26.25" customHeight="1">
+      <c r="A53" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correct previous added entry
</commit_message>
<xml_diff>
--- a/rpg_lib.xlsx
+++ b/rpg_lib.xlsx
@@ -1078,14 +1078,17 @@
     </r>
   </si>
   <si>
+    <t>%LOOKUP(CUXREL:VSOWNREL)
+When in array, retrun index number
+When not found, retrun a zero</t>
+  </si>
+  <si>
     <t>mylesDVSOWNREL         S              3    DIM(10) CTDATA
 …
 mylesC**             //program end
+** &lt;- this is the indicator of the start, not necessary to has 10 lines but these 2 stars are must
 SOW
 OWN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%LOOKUP(CUXREL:VSOWNREL) &lt;&gt; 0  </t>
   </si>
 </sst>
 </file>
@@ -1474,7 +1477,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1"/>
@@ -2055,7 +2058,7 @@
         <v>105</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="26.25" customHeight="1">
@@ -2066,7 +2069,7 @@
         <v>106</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="26.25" customHeight="1">

</xml_diff>